<commit_message>
campoos ok y subcampos presenta ma
</commit_message>
<xml_diff>
--- a/LecturaArchivos.xlsx
+++ b/LecturaArchivos.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="162">
+  <si>
+    <t>Cuenta</t>
+  </si>
   <si>
     <t>1001182818</t>
   </si>
@@ -22,37 +25,445 @@
     <t>1001182826</t>
   </si>
   <si>
-    <t>Cuenta</t>
+    <t>Moneda</t>
   </si>
   <si>
     <t>PEN</t>
   </si>
   <si>
-    <t>Moneda</t>
+    <t>campo2.3</t>
+  </si>
+  <si>
+    <t>TOTCOMMITMENT</t>
+  </si>
+  <si>
+    <t>campo2.4</t>
+  </si>
+  <si>
+    <t>CURCOMMITMENT</t>
+  </si>
+  <si>
+    <t>campo2.5</t>
+  </si>
+  <si>
+    <t>TOTCOMMITMENTBL</t>
+  </si>
+  <si>
+    <t>campo2.6</t>
+  </si>
+  <si>
+    <t>CURCOMMITMENTBL</t>
+  </si>
+  <si>
+    <t>campo2.7</t>
+  </si>
+  <si>
+    <t>AVLACCOUNT</t>
+  </si>
+  <si>
+    <t>campo2.8</t>
+  </si>
+  <si>
+    <t>AVLACCOUNTBL</t>
+  </si>
+  <si>
+    <t>campo2.9</t>
+  </si>
+  <si>
+    <t>CURACCOUNT</t>
+  </si>
+  <si>
+    <t>campo2.10</t>
+  </si>
+  <si>
+    <t>ACCPRINCIPALINT</t>
+  </si>
+  <si>
+    <t>campo2.11</t>
+  </si>
+  <si>
+    <t>AASUSPENSE</t>
+  </si>
+  <si>
+    <t>campo2.12</t>
+  </si>
+  <si>
+    <t>UNCACCOUNT</t>
+  </si>
+  <si>
+    <t>campo2.13</t>
+  </si>
+  <si>
+    <t>campo2.14</t>
+  </si>
+  <si>
+    <t>campo2.15</t>
+  </si>
+  <si>
+    <t>campo2.16</t>
+  </si>
+  <si>
+    <t>campo2.17</t>
+  </si>
+  <si>
+    <t>campo2.18</t>
+  </si>
+  <si>
+    <t>campo2.19</t>
+  </si>
+  <si>
+    <t>campo2.20</t>
+  </si>
+  <si>
+    <t>campo2.21</t>
+  </si>
+  <si>
+    <t>campo2.22</t>
+  </si>
+  <si>
+    <t>campo3.24</t>
+  </si>
+  <si>
+    <t>TOTCOMMITMENT-20200430</t>
+  </si>
+  <si>
+    <t>campo3.25</t>
+  </si>
+  <si>
+    <t>CURCOMMITMENT-20200430</t>
+  </si>
+  <si>
+    <t>campo3.26</t>
+  </si>
+  <si>
+    <t>TOTCOMMITMENTBL-20200430</t>
+  </si>
+  <si>
+    <t>campo3.27</t>
+  </si>
+  <si>
+    <t>CURCOMMITMENTBL-20200430</t>
+  </si>
+  <si>
+    <t>campo3.28</t>
+  </si>
+  <si>
+    <t>AVLACCOUNT-20200430</t>
+  </si>
+  <si>
+    <t>campo3.29</t>
+  </si>
+  <si>
+    <t>AVLACCOUNTBL-20200430</t>
+  </si>
+  <si>
+    <t>campo3.30</t>
+  </si>
+  <si>
+    <t>CURACCOUNT-20200430</t>
+  </si>
+  <si>
+    <t>campo3.31</t>
+  </si>
+  <si>
+    <t>ACCPRINCIPALINT-20200430</t>
+  </si>
+  <si>
+    <t>campo3.32</t>
+  </si>
+  <si>
+    <t>AASUSPENSE-20200430</t>
+  </si>
+  <si>
+    <t>campo3.33</t>
+  </si>
+  <si>
+    <t>UNCACCOUNT-20200430</t>
+  </si>
+  <si>
+    <t>campo3.34</t>
+  </si>
+  <si>
+    <t>campo3.35</t>
+  </si>
+  <si>
+    <t>campo3.36</t>
+  </si>
+  <si>
+    <t>campo3.37</t>
+  </si>
+  <si>
+    <t>campo3.38</t>
+  </si>
+  <si>
+    <t>campo3.39</t>
+  </si>
+  <si>
+    <t>campo3.40</t>
+  </si>
+  <si>
+    <t>campo3.41</t>
+  </si>
+  <si>
+    <t>campo3.42</t>
+  </si>
+  <si>
+    <t>campo3.43</t>
+  </si>
+  <si>
+    <t>campo4.45</t>
+  </si>
+  <si>
+    <t>campo4.46</t>
+  </si>
+  <si>
+    <t>campo4.47</t>
+  </si>
+  <si>
+    <t>campo4.48</t>
+  </si>
+  <si>
+    <t>campo4.49</t>
+  </si>
+  <si>
+    <t>campo4.50</t>
+  </si>
+  <si>
+    <t>campo4.51</t>
+  </si>
+  <si>
+    <t>campo4.52</t>
+  </si>
+  <si>
+    <t>campo4.53</t>
+  </si>
+  <si>
+    <t>campo4.54</t>
+  </si>
+  <si>
+    <t>campo4.55</t>
+  </si>
+  <si>
+    <t>campo4.56</t>
+  </si>
+  <si>
+    <t>campo4.57</t>
+  </si>
+  <si>
+    <t>campo4.58</t>
+  </si>
+  <si>
+    <t>campo4.59</t>
+  </si>
+  <si>
+    <t>campo4.60</t>
+  </si>
+  <si>
+    <t>campo4.61</t>
+  </si>
+  <si>
+    <t>campo4.62</t>
+  </si>
+  <si>
+    <t>campo4.63</t>
+  </si>
+  <si>
+    <t>campo4.64</t>
+  </si>
+  <si>
+    <t>campo5.66</t>
+  </si>
+  <si>
+    <t>-10474.66</t>
+  </si>
+  <si>
+    <t>campo5.67</t>
+  </si>
+  <si>
+    <t>-20949.32</t>
+  </si>
+  <si>
+    <t>campo5.68</t>
+  </si>
+  <si>
+    <t>campo5.69</t>
+  </si>
+  <si>
+    <t>campo5.70</t>
+  </si>
+  <si>
+    <t>campo5.71</t>
+  </si>
+  <si>
+    <t>campo5.72</t>
+  </si>
+  <si>
+    <t>-10080.64</t>
+  </si>
+  <si>
+    <t>campo5.73</t>
+  </si>
+  <si>
+    <t>-219.65</t>
+  </si>
+  <si>
+    <t>campo5.74</t>
+  </si>
+  <si>
+    <t>-0.06</t>
+  </si>
+  <si>
+    <t>campo5.75</t>
+  </si>
+  <si>
+    <t>campo5.76</t>
+  </si>
+  <si>
+    <t>-10193.75</t>
+  </si>
+  <si>
+    <t>campo5.77</t>
+  </si>
+  <si>
+    <t>-20387.5</t>
+  </si>
+  <si>
+    <t>campo5.78</t>
+  </si>
+  <si>
+    <t>campo5.79</t>
+  </si>
+  <si>
+    <t>campo5.80</t>
+  </si>
+  <si>
+    <t>campo5.81</t>
+  </si>
+  <si>
+    <t>campo5.82</t>
+  </si>
+  <si>
+    <t>-9810.29</t>
+  </si>
+  <si>
+    <t>campo5.83</t>
+  </si>
+  <si>
+    <t>-213.76</t>
+  </si>
+  <si>
+    <t>campo5.84</t>
+  </si>
+  <si>
+    <t>-0.04</t>
+  </si>
+  <si>
+    <t>campo5.85</t>
+  </si>
+  <si>
+    <t>campo6.87</t>
+  </si>
+  <si>
+    <t>campo6.88</t>
+  </si>
+  <si>
+    <t>20949.32</t>
+  </si>
+  <si>
+    <t>campo6.89</t>
+  </si>
+  <si>
+    <t>10474.66</t>
+  </si>
+  <si>
+    <t>campo6.90</t>
+  </si>
+  <si>
+    <t>campo6.91</t>
+  </si>
+  <si>
+    <t>campo6.92</t>
+  </si>
+  <si>
+    <t>campo6.93</t>
+  </si>
+  <si>
+    <t>campo6.94</t>
+  </si>
+  <si>
+    <t>campo6.95</t>
+  </si>
+  <si>
+    <t>0.06</t>
+  </si>
+  <si>
+    <t>campo6.96</t>
+  </si>
+  <si>
+    <t>campo6.97</t>
+  </si>
+  <si>
+    <t>campo6.98</t>
+  </si>
+  <si>
+    <t>20387.5</t>
+  </si>
+  <si>
+    <t>campo6.99</t>
+  </si>
+  <si>
+    <t>10193.75</t>
+  </si>
+  <si>
+    <t>campo6.100</t>
+  </si>
+  <si>
+    <t>campo6.101</t>
+  </si>
+  <si>
+    <t>campo6.102</t>
+  </si>
+  <si>
+    <t>campo6.103</t>
+  </si>
+  <si>
+    <t>campo6.104</t>
+  </si>
+  <si>
+    <t>campo6.105</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>campo6.106</t>
+  </si>
+  <si>
+    <t>FieldName3</t>
   </si>
   <si>
     <t>PE0010001</t>
   </si>
   <si>
-    <t>FieldName3</t>
+    <t>FieldName4</t>
   </si>
   <si>
     <t>ACCOUNT</t>
   </si>
   <si>
-    <t>FieldName4</t>
+    <t>FieldName5</t>
   </si>
   <si>
     <t>AC</t>
   </si>
   <si>
-    <t>FieldName5</t>
+    <t>FieldName6</t>
   </si>
   <si>
     <t>20200430</t>
   </si>
   <si>
-    <t>FieldName6</t>
+    <t>FieldName7</t>
   </si>
   <si>
     <t>3271222</t>
@@ -61,7 +472,7 @@
     <t>2236327</t>
   </si>
   <si>
-    <t>FieldName7</t>
+    <t>FieldName8</t>
   </si>
   <si>
     <t>-10080.58</t>
@@ -70,22 +481,22 @@
     <t>-9810.25</t>
   </si>
   <si>
-    <t>FieldName8</t>
-  </si>
-  <si>
     <t>FieldName9</t>
   </si>
   <si>
+    <t>FieldName10</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
-    <t>FieldName10</t>
-  </si>
-  <si>
     <t>13:45:56 30 APR 2020</t>
   </si>
   <si>
     <t>13:53:06 30 APR 2020</t>
+  </si>
+  <si>
+    <t>FieldValue11</t>
   </si>
   <si>
     <t>AC.1.TR.PEN.3132.1001.PE.5Y.10..1001......PE0010001</t>
@@ -420,121 +831,634 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:DM3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:117">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>104</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>105</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>106</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>107</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>108</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>110</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>112</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>114</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>115</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>116</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>118</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>120</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>121</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>122</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>123</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>125</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>127</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>128</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>129</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>131</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>133</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>134</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>135</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>136</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>137</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>138</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>140</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>141</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>143</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>145</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>147</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>149</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>152</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>155</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>156</v>
+      </c>
+      <c r="DL1" t="s">
+        <v>156</v>
+      </c>
+      <c r="DM1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:117">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>88</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>88</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>88</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>88</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>94</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>96</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>98</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>103</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>103</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>103</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>103</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>109</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>111</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>113</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>117</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>119</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>117</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>117</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>117</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>126</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>126</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>130</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>132</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>130</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>130</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>130</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>139</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>139</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>142</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>144</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>146</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>148</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>150</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>153</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>153</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>157</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>158</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:117">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" t="s">
-        <v>17</v>
-      </c>
       <c r="N3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>24</v>
+        <v>6</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>36</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>86</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>101</v>
+      </c>
+      <c r="DD3" t="s">
+        <v>142</v>
+      </c>
+      <c r="DE3" t="s">
+        <v>144</v>
+      </c>
+      <c r="DF3" t="s">
+        <v>146</v>
+      </c>
+      <c r="DG3" t="s">
+        <v>148</v>
+      </c>
+      <c r="DH3" t="s">
+        <v>151</v>
+      </c>
+      <c r="DI3" t="s">
+        <v>154</v>
+      </c>
+      <c r="DJ3" t="s">
+        <v>154</v>
+      </c>
+      <c r="DK3" t="s">
+        <v>157</v>
+      </c>
+      <c r="DL3" t="s">
+        <v>159</v>
+      </c>
+      <c r="DM3" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>